<commit_message>
edit all scripts to update excle
</commit_message>
<xml_diff>
--- a/new_data/pathways.xlsx
+++ b/new_data/pathways.xlsx
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,9 +1141,15 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
@@ -1161,9 +1167,15 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
@@ -1181,9 +1193,15 @@
       <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
@@ -1201,9 +1219,15 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
       <c r="G5" s="11"/>
       <c r="H5" s="5"/>
       <c r="I5" s="15"/>
@@ -1221,9 +1245,15 @@
       <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="5"/>
       <c r="I6" s="15"/>
@@ -1241,9 +1271,15 @@
       <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
       <c r="G7" s="11"/>
       <c r="H7" s="5"/>
       <c r="I7" s="15"/>
@@ -1261,9 +1297,15 @@
       <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
       <c r="G8" s="11"/>
       <c r="H8" s="5"/>
       <c r="I8" s="15"/>
@@ -1281,9 +1323,15 @@
       <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="5"/>
       <c r="I9" s="15"/>
@@ -1301,9 +1349,15 @@
       <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
       <c r="G10" s="11"/>
       <c r="H10" s="5"/>
       <c r="I10" s="15"/>
@@ -1321,9 +1375,15 @@
       <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="5"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="5"/>
       <c r="I11" s="15"/>
@@ -1341,9 +1401,15 @@
       <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="5"/>
       <c r="I12" s="15"/>
@@ -1361,9 +1427,15 @@
       <c r="C13" s="11">
         <v>1</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
       <c r="G13" s="11"/>
       <c r="H13" s="5"/>
       <c r="I13" s="15"/>
@@ -1417,9 +1489,15 @@
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
@@ -1437,9 +1515,15 @@
       <c r="C17" s="11">
         <v>1</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="5"/>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="5"/>
       <c r="I17" s="15"/>
@@ -1457,9 +1541,15 @@
       <c r="C18" s="11">
         <v>1</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
       <c r="G18" s="11"/>
       <c r="H18" s="5"/>
       <c r="I18" s="15"/>
@@ -1477,9 +1567,15 @@
       <c r="C19" s="11">
         <v>1</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="5"/>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="5"/>
       <c r="I19" s="15"/>
@@ -1497,9 +1593,15 @@
       <c r="C20" s="11">
         <v>1</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="5"/>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
       <c r="G20" s="11"/>
       <c r="H20" s="5"/>
       <c r="I20" s="15"/>
@@ -1517,9 +1619,15 @@
       <c r="C21" s="11">
         <v>1</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="5"/>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
       <c r="G21" s="11"/>
       <c r="H21" s="5"/>
       <c r="I21" s="15"/>
@@ -1537,9 +1645,15 @@
       <c r="C22" s="11">
         <v>1</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="5"/>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
       <c r="G22" s="11"/>
       <c r="H22" s="5"/>
       <c r="I22" s="15"/>
@@ -1557,9 +1671,15 @@
       <c r="C23" s="11">
         <v>1</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="5"/>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
       <c r="G23" s="11"/>
       <c r="H23" s="5"/>
       <c r="I23" s="15"/>
@@ -1577,9 +1697,15 @@
       <c r="C24" s="11">
         <v>1</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="5"/>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
       <c r="G24" s="11"/>
       <c r="H24" s="5"/>
       <c r="I24" s="15"/>
@@ -1597,9 +1723,15 @@
       <c r="C25" s="11">
         <v>1</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="5"/>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
       <c r="G25" s="11"/>
       <c r="H25" s="5"/>
       <c r="I25" s="15"/>
@@ -1617,9 +1749,15 @@
       <c r="C26" s="11">
         <v>1</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="5"/>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
       <c r="G26" s="11"/>
       <c r="H26" s="5"/>
       <c r="I26" s="15"/>
@@ -1634,10 +1772,18 @@
       <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="6"/>
@@ -1688,10 +1834,18 @@
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
@@ -1709,9 +1863,15 @@
       <c r="C31" s="5">
         <v>1</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="6"/>
@@ -1726,10 +1886,18 @@
       <c r="B32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="6"/>
@@ -1945,9 +2113,15 @@
       <c r="C44" s="2">
         <v>1</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="3"/>
@@ -1962,10 +2136,18 @@
       <c r="B45" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="6"/>
@@ -1980,10 +2162,18 @@
       <c r="B46" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="C46" s="5">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5">
+        <v>1</v>
+      </c>
+      <c r="E46" s="5">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>1</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
@@ -2214,10 +2404,18 @@
       <c r="B59" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
+      <c r="C59" s="5">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5">
+        <v>1</v>
+      </c>
+      <c r="E59" s="5">
+        <v>1</v>
+      </c>
+      <c r="F59" s="5">
+        <v>1</v>
+      </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="6"/>
@@ -2448,10 +2646,18 @@
       <c r="B72" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
+      <c r="C72" s="2">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2">
+        <v>1</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="3"/>
@@ -2466,10 +2672,18 @@
       <c r="B73" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="C73" s="5">
+        <v>1</v>
+      </c>
+      <c r="D73" s="5">
+        <v>1</v>
+      </c>
+      <c r="E73" s="5">
+        <v>1</v>
+      </c>
+      <c r="F73" s="5">
+        <v>1</v>
+      </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="6"/>

</xml_diff>

<commit_message>
Bug fixes to processing files, and latest version of Pathways file
</commit_message>
<xml_diff>
--- a/new_data/pathways.xlsx
+++ b/new_data/pathways.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="32">
   <si>
     <t>mouse</t>
   </si>
@@ -43,60 +43,6 @@
     <t>Motion_correction</t>
   </si>
   <si>
-    <t>day_1</t>
-  </si>
-  <si>
-    <t>day_3</t>
-  </si>
-  <si>
-    <t>day_5</t>
-  </si>
-  <si>
-    <t>day_7</t>
-  </si>
-  <si>
-    <t>day_9</t>
-  </si>
-  <si>
-    <t>day_11</t>
-  </si>
-  <si>
-    <t>day_13</t>
-  </si>
-  <si>
-    <t>day_15A</t>
-  </si>
-  <si>
-    <t>day_19L</t>
-  </si>
-  <si>
-    <t>day_30A</t>
-  </si>
-  <si>
-    <t>day_34L</t>
-  </si>
-  <si>
-    <t>day_2</t>
-  </si>
-  <si>
-    <t>day_4</t>
-  </si>
-  <si>
-    <t>day_6</t>
-  </si>
-  <si>
-    <t>day_8</t>
-  </si>
-  <si>
-    <t>day_10</t>
-  </si>
-  <si>
-    <t>day_12</t>
-  </si>
-  <si>
-    <t>day_14</t>
-  </si>
-  <si>
     <t>BaselineS</t>
   </si>
   <si>
@@ -110,6 +56,60 @@
   </si>
   <si>
     <t>BaslineS</t>
+  </si>
+  <si>
+    <t>day1</t>
+  </si>
+  <si>
+    <t>day3</t>
+  </si>
+  <si>
+    <t>day5</t>
+  </si>
+  <si>
+    <t>day7</t>
+  </si>
+  <si>
+    <t>day9</t>
+  </si>
+  <si>
+    <t>day11</t>
+  </si>
+  <si>
+    <t>day13</t>
+  </si>
+  <si>
+    <t>day15A</t>
+  </si>
+  <si>
+    <t>day19L</t>
+  </si>
+  <si>
+    <t>day30A</t>
+  </si>
+  <si>
+    <t>day34L</t>
+  </si>
+  <si>
+    <t>day2</t>
+  </si>
+  <si>
+    <t>day4</t>
+  </si>
+  <si>
+    <t>day6</t>
+  </si>
+  <si>
+    <t>day8</t>
+  </si>
+  <si>
+    <t>day10</t>
+  </si>
+  <si>
+    <t>day12</t>
+  </si>
+  <si>
+    <t>day14</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>8</v>
@@ -1136,7 +1136,7 @@
         <v>1236</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1150,11 +1150,15 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1162,7 +1166,7 @@
         <v>1236</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -1176,11 +1180,15 @@
       <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1188,7 +1196,7 @@
         <v>1236</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1202,11 +1210,15 @@
       <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1214,7 +1226,7 @@
         <v>1236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -1228,11 +1240,15 @@
       <c r="F5" s="5">
         <v>1</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
       <c r="I5" s="15"/>
       <c r="J5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1240,7 +1256,7 @@
         <v>1236</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="11">
         <v>1</v>
@@ -1254,11 +1270,15 @@
       <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
       <c r="I6" s="15"/>
       <c r="J6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1266,7 +1286,7 @@
         <v>1236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
@@ -1280,11 +1300,15 @@
       <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
       <c r="I7" s="15"/>
       <c r="J7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1292,7 +1316,7 @@
         <v>1236</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C8" s="11">
         <v>1</v>
@@ -1306,11 +1330,15 @@
       <c r="F8" s="5">
         <v>1</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1318,7 +1346,7 @@
         <v>1236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="11">
         <v>1</v>
@@ -1332,11 +1360,15 @@
       <c r="F9" s="5">
         <v>1</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
       <c r="I9" s="15"/>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1344,7 +1376,7 @@
         <v>1236</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -1358,11 +1390,15 @@
       <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="5"/>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
       <c r="I10" s="15"/>
       <c r="J10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,7 +1406,7 @@
         <v>1236</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
@@ -1384,11 +1420,15 @@
       <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
       <c r="I11" s="15"/>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1396,7 +1436,7 @@
         <v>1236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C12" s="11">
         <v>1</v>
@@ -1410,11 +1450,15 @@
       <c r="F12" s="5">
         <v>1</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
       <c r="I12" s="15"/>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1422,7 +1466,7 @@
         <v>1236</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C13" s="11">
         <v>1</v>
@@ -1436,11 +1480,15 @@
       <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="5"/>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
       <c r="I13" s="15"/>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1448,17 +1496,29 @@
         <v>1236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1466,7 +1526,7 @@
         <v>1236</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1476,7 +1536,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1484,7 +1544,7 @@
         <v>8430</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -1498,11 +1558,13 @@
       <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
       <c r="J16" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1510,7 +1572,7 @@
         <v>8430</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C17" s="11">
         <v>1</v>
@@ -1524,11 +1586,15 @@
       <c r="F17" s="5">
         <v>1</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
       <c r="I17" s="15"/>
       <c r="J17" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1536,7 +1602,7 @@
         <v>8430</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
@@ -1550,11 +1616,15 @@
       <c r="F18" s="5">
         <v>1</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
       <c r="I18" s="15"/>
       <c r="J18" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1562,7 +1632,7 @@
         <v>8430</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C19" s="11">
         <v>1</v>
@@ -1576,11 +1646,15 @@
       <c r="F19" s="5">
         <v>1</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
       <c r="I19" s="15"/>
       <c r="J19" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1588,7 +1662,7 @@
         <v>8430</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C20" s="11">
         <v>1</v>
@@ -1602,11 +1676,15 @@
       <c r="F20" s="5">
         <v>1</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
       <c r="I20" s="15"/>
       <c r="J20" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1614,7 +1692,7 @@
         <v>8430</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C21" s="11">
         <v>1</v>
@@ -1629,10 +1707,12 @@
         <v>1</v>
       </c>
       <c r="G21" s="11"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
       <c r="I21" s="15"/>
       <c r="J21" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1640,7 +1720,7 @@
         <v>8430</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C22" s="11">
         <v>1</v>
@@ -1654,11 +1734,15 @@
       <c r="F22" s="5">
         <v>1</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="11">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
       <c r="I22" s="15"/>
       <c r="J22" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1666,7 +1750,7 @@
         <v>8430</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C23" s="11">
         <v>1</v>
@@ -1680,11 +1764,15 @@
       <c r="F23" s="5">
         <v>1</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="11">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
       <c r="I23" s="15"/>
       <c r="J23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1692,7 +1780,7 @@
         <v>8430</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C24" s="11">
         <v>1</v>
@@ -1706,11 +1794,15 @@
       <c r="F24" s="5">
         <v>1</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="11">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
       <c r="I24" s="15"/>
       <c r="J24" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1718,7 +1810,7 @@
         <v>8430</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C25" s="11">
         <v>1</v>
@@ -1732,11 +1824,15 @@
       <c r="F25" s="5">
         <v>1</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
       <c r="I25" s="15"/>
       <c r="J25" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1744,7 +1840,7 @@
         <v>8430</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
@@ -1758,11 +1854,15 @@
       <c r="F26" s="5">
         <v>1</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
       <c r="I26" s="15"/>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1770,7 +1870,7 @@
         <v>8430</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -1784,11 +1884,15 @@
       <c r="F27" s="5">
         <v>1</v>
       </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
       <c r="I27" s="6"/>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1796,17 +1900,29 @@
         <v>8430</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
       <c r="I28" s="6"/>
       <c r="J28" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1814,7 +1930,7 @@
         <v>8430</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -1824,7 +1940,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="9"/>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1832,7 +1948,7 @@
         <v>8815</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -1846,11 +1962,15 @@
       <c r="F30" s="2">
         <v>1</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
       <c r="I30" s="3"/>
       <c r="J30" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1858,7 +1978,7 @@
         <v>8815</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
@@ -1872,11 +1992,15 @@
       <c r="F31" s="5">
         <v>1</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
       <c r="I31" s="6"/>
       <c r="J31" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1884,7 +2008,7 @@
         <v>8815</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -1898,11 +2022,13 @@
       <c r="F32" s="5">
         <v>1</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
       <c r="H32" s="5"/>
       <c r="I32" s="6"/>
       <c r="J32" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1910,17 +2036,29 @@
         <v>8815</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
       <c r="I33" s="6"/>
       <c r="J33" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1928,17 +2066,29 @@
         <v>8815</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1</v>
+      </c>
       <c r="I34" s="6"/>
       <c r="J34" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1946,17 +2096,29 @@
         <v>8815</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1</v>
+      </c>
       <c r="I35" s="6"/>
       <c r="J35" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1964,17 +2126,29 @@
         <v>8815</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
       <c r="I36" s="6"/>
       <c r="J36" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1982,17 +2156,29 @@
         <v>8815</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5">
+        <v>1</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1</v>
+      </c>
       <c r="I37" s="6"/>
       <c r="J37" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2000,17 +2186,29 @@
         <v>8815</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
       <c r="I38" s="6"/>
       <c r="J38" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2018,17 +2216,29 @@
         <v>8815</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5">
+        <v>1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1</v>
+      </c>
       <c r="I39" s="6"/>
       <c r="J39" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2036,17 +2246,21 @@
         <v>8815</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
       <c r="H40" s="5"/>
       <c r="I40" s="6"/>
       <c r="J40" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2054,7 +2268,7 @@
         <v>8815</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -2064,7 +2278,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="6"/>
       <c r="J41" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2072,7 +2286,7 @@
         <v>8815</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -2082,7 +2296,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="6"/>
       <c r="J42" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2090,7 +2304,7 @@
         <v>8815</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -2100,7 +2314,7 @@
       <c r="H43" s="8"/>
       <c r="I43" s="9"/>
       <c r="J43" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2108,7 +2322,7 @@
         <v>8803</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -2122,11 +2336,15 @@
       <c r="F44" s="2">
         <v>1</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="G44" s="2">
+        <v>1</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="J44" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2134,7 +2352,7 @@
         <v>8803</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C45" s="5">
         <v>1</v>
@@ -2148,11 +2366,15 @@
       <c r="F45" s="5">
         <v>1</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
       <c r="I45" s="6"/>
       <c r="J45" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2160,7 +2382,7 @@
         <v>8803</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C46" s="5">
         <v>1</v>
@@ -2174,11 +2396,13 @@
       <c r="F46" s="5">
         <v>1</v>
       </c>
-      <c r="G46" s="5"/>
+      <c r="G46" s="5">
+        <v>1</v>
+      </c>
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
       <c r="J46" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2186,17 +2410,29 @@
         <v>8803</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1</v>
+      </c>
+      <c r="E47" s="5">
+        <v>1</v>
+      </c>
+      <c r="F47" s="5">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5">
+        <v>1</v>
+      </c>
       <c r="I47" s="6"/>
       <c r="J47" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2204,17 +2440,29 @@
         <v>8803</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C48" s="5">
+        <v>1</v>
+      </c>
+      <c r="D48" s="5">
+        <v>1</v>
+      </c>
+      <c r="E48" s="5">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1</v>
+      </c>
       <c r="I48" s="6"/>
       <c r="J48" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2222,17 +2470,25 @@
         <v>8803</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5">
+        <v>1</v>
+      </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="G49" s="5">
+        <v>1</v>
+      </c>
+      <c r="H49" s="5">
+        <v>1</v>
+      </c>
       <c r="I49" s="6"/>
       <c r="J49" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2240,17 +2496,29 @@
         <v>8803</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5">
+        <v>1</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1</v>
+      </c>
+      <c r="H50" s="5">
+        <v>1</v>
+      </c>
       <c r="I50" s="6"/>
       <c r="J50" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2258,17 +2526,29 @@
         <v>8803</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1</v>
+      </c>
+      <c r="E51" s="5">
+        <v>1</v>
+      </c>
+      <c r="F51" s="5">
+        <v>1</v>
+      </c>
+      <c r="G51" s="5">
+        <v>1</v>
+      </c>
+      <c r="H51" s="5">
+        <v>1</v>
+      </c>
       <c r="I51" s="6"/>
       <c r="J51" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2276,17 +2556,29 @@
         <v>8803</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5">
+        <v>1</v>
+      </c>
+      <c r="E52" s="5">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5">
+        <v>1</v>
+      </c>
+      <c r="G52" s="5">
+        <v>1</v>
+      </c>
+      <c r="H52" s="5">
+        <v>1</v>
+      </c>
       <c r="I52" s="6"/>
       <c r="J52" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2294,35 +2586,59 @@
         <v>8803</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1</v>
+      </c>
+      <c r="E53" s="5">
+        <v>1</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1</v>
+      </c>
+      <c r="G53" s="5">
+        <v>1</v>
+      </c>
+      <c r="H53" s="5">
+        <v>1</v>
+      </c>
       <c r="I53" s="6"/>
       <c r="J53" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>8803</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="B54" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1</v>
+      </c>
+      <c r="E54" s="5">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5">
+        <v>1</v>
+      </c>
+      <c r="G54" s="5">
+        <v>1</v>
+      </c>
+      <c r="H54" s="5">
+        <v>1</v>
+      </c>
       <c r="I54" s="6"/>
       <c r="J54" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2330,17 +2646,19 @@
         <v>8803</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="G55" s="5">
+        <v>1</v>
+      </c>
       <c r="H55" s="5"/>
       <c r="I55" s="6"/>
       <c r="J55" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2348,7 +2666,7 @@
         <v>8803</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -2358,69 +2676,73 @@
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="12">
         <v>8803</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="9"/>
+      <c r="B57" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="6"/>
       <c r="J57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
+        <v>8803</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="9"/>
+      <c r="J58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="13">
         <v>1208</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="3"/>
-      <c r="J58" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="12">
-        <v>1208</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59" s="5">
-        <v>1</v>
-      </c>
-      <c r="D59" s="5">
-        <v>1</v>
-      </c>
-      <c r="E59" s="5">
-        <v>1</v>
-      </c>
-      <c r="F59" s="5">
-        <v>1</v>
-      </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="6"/>
+      <c r="B59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1</v>
+      </c>
+      <c r="I59" s="3"/>
       <c r="J59" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2428,35 +2750,59 @@
         <v>1208</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1</v>
+      </c>
+      <c r="D60" s="5">
+        <v>1</v>
+      </c>
+      <c r="E60" s="5">
+        <v>1</v>
+      </c>
+      <c r="F60" s="5">
+        <v>1</v>
+      </c>
+      <c r="G60" s="5">
+        <v>1</v>
+      </c>
+      <c r="H60" s="5">
+        <v>1</v>
+      </c>
       <c r="I60" s="6"/>
       <c r="J60" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>1208</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="B61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1</v>
+      </c>
+      <c r="E61" s="5">
+        <v>1</v>
+      </c>
+      <c r="F61" s="5">
+        <v>1</v>
+      </c>
+      <c r="G61" s="5">
+        <v>1</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1</v>
+      </c>
       <c r="I61" s="6"/>
       <c r="J61" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2464,17 +2810,29 @@
         <v>1208</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1</v>
+      </c>
+      <c r="E62" s="5">
+        <v>1</v>
+      </c>
+      <c r="F62" s="5">
+        <v>1</v>
+      </c>
+      <c r="G62" s="5">
+        <v>1</v>
+      </c>
+      <c r="H62" s="5">
+        <v>1</v>
+      </c>
       <c r="I62" s="6"/>
       <c r="J62" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -2482,17 +2840,29 @@
         <v>1208</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1</v>
+      </c>
+      <c r="E63" s="5">
+        <v>1</v>
+      </c>
+      <c r="F63" s="5">
+        <v>1</v>
+      </c>
+      <c r="G63" s="5">
+        <v>1</v>
+      </c>
+      <c r="H63" s="5">
+        <v>1</v>
+      </c>
       <c r="I63" s="6"/>
       <c r="J63" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2500,17 +2870,29 @@
         <v>1208</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1</v>
+      </c>
+      <c r="E64" s="5">
+        <v>1</v>
+      </c>
+      <c r="F64" s="5">
+        <v>1</v>
+      </c>
+      <c r="G64" s="5">
+        <v>1</v>
+      </c>
+      <c r="H64" s="5">
+        <v>1</v>
+      </c>
       <c r="I64" s="6"/>
       <c r="J64" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2518,9 +2900,11 @@
         <v>1208</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C65" s="5">
+        <v>1</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -2528,7 +2912,7 @@
       <c r="H65" s="5"/>
       <c r="I65" s="6"/>
       <c r="J65" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2536,9 +2920,11 @@
         <v>1208</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C66" s="5">
+        <v>1</v>
+      </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -2546,7 +2932,7 @@
       <c r="H66" s="5"/>
       <c r="I66" s="6"/>
       <c r="J66" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2554,7 +2940,7 @@
         <v>1208</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2564,15 +2950,15 @@
       <c r="H67" s="5"/>
       <c r="I67" s="6"/>
       <c r="J67" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>1208</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>16</v>
+      <c r="B68" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2582,7 +2968,7 @@
       <c r="H68" s="5"/>
       <c r="I68" s="6"/>
       <c r="J68" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2590,7 +2976,7 @@
         <v>1208</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -2600,7 +2986,7 @@
       <c r="H69" s="5"/>
       <c r="I69" s="6"/>
       <c r="J69" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -2608,7 +2994,7 @@
         <v>1208</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2618,77 +3004,73 @@
       <c r="H70" s="5"/>
       <c r="I70" s="6"/>
       <c r="J70" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="12">
         <v>1208</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="9"/>
+      <c r="B71" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="6"/>
       <c r="J71" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="14">
+        <v>1208</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="9"/>
+      <c r="J72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="13">
         <v>1793</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" s="2">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2">
-        <v>1</v>
-      </c>
-      <c r="F72" s="2">
-        <v>1</v>
-      </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="3"/>
-      <c r="J72" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="12">
-        <v>1793</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C73" s="5">
-        <v>1</v>
-      </c>
-      <c r="D73" s="5">
-        <v>1</v>
-      </c>
-      <c r="E73" s="5">
-        <v>1</v>
-      </c>
-      <c r="F73" s="5">
-        <v>1</v>
-      </c>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="6"/>
+      <c r="B73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1</v>
+      </c>
+      <c r="G73" s="2">
+        <v>1</v>
+      </c>
+      <c r="H73" s="2">
+        <v>1</v>
+      </c>
+      <c r="I73" s="3"/>
       <c r="J73" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2696,35 +3078,55 @@
         <v>1793</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1</v>
+      </c>
+      <c r="D74" s="5">
+        <v>1</v>
+      </c>
+      <c r="E74" s="5">
+        <v>1</v>
+      </c>
+      <c r="F74" s="5">
+        <v>1</v>
+      </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="6"/>
       <c r="J74" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>1793</v>
       </c>
-      <c r="B75" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
+      <c r="B75" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5">
+        <v>1</v>
+      </c>
+      <c r="E75" s="5">
+        <v>1</v>
+      </c>
+      <c r="F75" s="5">
+        <v>1</v>
+      </c>
+      <c r="G75" s="5">
+        <v>1</v>
+      </c>
+      <c r="H75" s="5">
+        <v>1</v>
+      </c>
       <c r="I75" s="6"/>
       <c r="J75" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2732,17 +3134,29 @@
         <v>1793</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C76" s="5">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5">
+        <v>1</v>
+      </c>
+      <c r="E76" s="5">
+        <v>1</v>
+      </c>
+      <c r="F76" s="5">
+        <v>1</v>
+      </c>
+      <c r="G76" s="5">
+        <v>1</v>
+      </c>
+      <c r="H76" s="5">
+        <v>1</v>
+      </c>
       <c r="I76" s="6"/>
       <c r="J76" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2750,17 +3164,29 @@
         <v>1793</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C77" s="5">
+        <v>1</v>
+      </c>
+      <c r="D77" s="5">
+        <v>1</v>
+      </c>
+      <c r="E77" s="5">
+        <v>1</v>
+      </c>
+      <c r="F77" s="5">
+        <v>1</v>
+      </c>
+      <c r="G77" s="5">
+        <v>1</v>
+      </c>
+      <c r="H77" s="5">
+        <v>1</v>
+      </c>
       <c r="I77" s="6"/>
       <c r="J77" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -2768,17 +3194,27 @@
         <v>1793</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C78" s="5">
+        <v>1</v>
+      </c>
+      <c r="D78" s="5">
+        <v>1</v>
+      </c>
+      <c r="E78" s="5">
+        <v>1</v>
+      </c>
+      <c r="F78" s="5">
+        <v>1</v>
+      </c>
       <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
+      <c r="H78" s="5">
+        <v>1</v>
+      </c>
       <c r="I78" s="6"/>
       <c r="J78" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2786,9 +3222,11 @@
         <v>1793</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C79" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C79" s="5">
+        <v>1</v>
+      </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
@@ -2796,7 +3234,7 @@
       <c r="H79" s="5"/>
       <c r="I79" s="6"/>
       <c r="J79" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2804,9 +3242,11 @@
         <v>1793</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C80" s="5">
+        <v>1</v>
+      </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -2814,7 +3254,7 @@
       <c r="H80" s="5"/>
       <c r="I80" s="6"/>
       <c r="J80" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -2822,7 +3262,7 @@
         <v>1793</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -2832,15 +3272,15 @@
       <c r="H81" s="5"/>
       <c r="I81" s="6"/>
       <c r="J81" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>1793</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>16</v>
+      <c r="B82" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -2850,7 +3290,7 @@
       <c r="H82" s="5"/>
       <c r="I82" s="6"/>
       <c r="J82" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -2858,7 +3298,7 @@
         <v>1793</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -2868,7 +3308,7 @@
       <c r="H83" s="5"/>
       <c r="I83" s="6"/>
       <c r="J83" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -2876,7 +3316,7 @@
         <v>1793</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -2886,25 +3326,43 @@
       <c r="H84" s="5"/>
       <c r="I84" s="6"/>
       <c r="J84" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="12">
         <v>1793</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="9"/>
+      <c r="B85" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="6"/>
       <c r="J85" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="14">
+        <v>1793</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="9"/>
+      <c r="J86" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new scripts and updates xlsx
</commit_message>
<xml_diff>
--- a/new_data/pathways.xlsx
+++ b/new_data/pathways.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="39">
   <si>
     <t>mouse</t>
   </si>
@@ -115,9 +115,6 @@
     <t>day35L</t>
   </si>
   <si>
-    <t>day19</t>
-  </si>
-  <si>
     <t>ROI_check</t>
   </si>
   <si>
@@ -125,6 +122,15 @@
   </si>
   <si>
     <t>re_extract</t>
+  </si>
+  <si>
+    <t>maxloc</t>
+  </si>
+  <si>
+    <t>handScore</t>
+  </si>
+  <si>
+    <t>hs_t</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,13 +1120,16 @@
     <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1146,22 +1155,31 @@
         <v>5</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="M1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1236</v>
       </c>
@@ -1177,7 +1195,9 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
       <c r="G2" s="2">
         <v>1</v>
       </c>
@@ -1187,16 +1207,23 @@
       <c r="I2" s="2">
         <v>637</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" t="s">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1236</v>
       </c>
@@ -1212,7 +1239,9 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
       <c r="G3" s="5">
         <v>1</v>
       </c>
@@ -1222,16 +1251,23 @@
       <c r="I3" s="5">
         <v>262</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
       <c r="K3" s="5">
         <v>1</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1236</v>
       </c>
@@ -1247,7 +1283,9 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
       <c r="G4" s="5">
         <v>1</v>
       </c>
@@ -1257,16 +1295,23 @@
       <c r="I4" s="5">
         <v>503</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
       <c r="K4" s="5">
         <v>1</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1236</v>
       </c>
@@ -1282,7 +1327,9 @@
       <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
       <c r="G5" s="11">
         <v>1</v>
       </c>
@@ -1292,16 +1339,23 @@
       <c r="I5" s="5">
         <v>350</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
       <c r="K5" s="5">
         <v>1</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" t="s">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="15"/>
+      <c r="P5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1236</v>
       </c>
@@ -1317,7 +1371,9 @@
       <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
       <c r="G6" s="11">
         <v>1</v>
       </c>
@@ -1327,16 +1383,23 @@
       <c r="I6" s="5">
         <v>270</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
       <c r="K6" s="5">
         <v>1</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5">
+        <v>1</v>
+      </c>
+      <c r="O6" s="15"/>
+      <c r="P6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1236</v>
       </c>
@@ -1352,7 +1415,9 @@
       <c r="E7" s="11">
         <v>1</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
       <c r="G7" s="11">
         <v>1</v>
       </c>
@@ -1362,16 +1427,23 @@
       <c r="I7" s="5">
         <v>199</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
       <c r="K7" s="5">
         <v>1</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" t="s">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5">
+        <v>1</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1236</v>
       </c>
@@ -1387,7 +1459,9 @@
       <c r="E8" s="11">
         <v>1</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
       <c r="G8" s="11">
         <v>1</v>
       </c>
@@ -1397,16 +1471,23 @@
       <c r="I8" s="5">
         <v>112</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
       <c r="K8" s="5">
         <v>1</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" t="s">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="15"/>
+      <c r="P8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1236</v>
       </c>
@@ -1422,7 +1503,9 @@
       <c r="E9" s="11">
         <v>1</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="G9" s="11">
         <v>1</v>
       </c>
@@ -1432,16 +1515,23 @@
       <c r="I9" s="5">
         <v>153</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
       <c r="K9" s="5">
         <v>1</v>
       </c>
-      <c r="L9" s="15"/>
-      <c r="M9" t="s">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="15"/>
+      <c r="P9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1236</v>
       </c>
@@ -1457,7 +1547,9 @@
       <c r="E10" s="11">
         <v>1</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
       <c r="G10" s="11">
         <v>1</v>
       </c>
@@ -1467,16 +1559,23 @@
       <c r="I10" s="5">
         <v>196</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
       <c r="K10" s="5">
         <v>1</v>
       </c>
-      <c r="L10" s="15"/>
-      <c r="M10" t="s">
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5">
+        <v>1</v>
+      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1236</v>
       </c>
@@ -1492,7 +1591,9 @@
       <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
       <c r="G11" s="11">
         <v>1</v>
       </c>
@@ -1502,16 +1603,23 @@
       <c r="I11" s="5">
         <v>239</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
       <c r="K11" s="5">
         <v>1</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" t="s">
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5">
+        <v>1</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1236</v>
       </c>
@@ -1536,15 +1644,26 @@
       <c r="H12" s="5">
         <v>1</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="15"/>
-      <c r="M12" t="s">
+      <c r="I12" s="5">
+        <v>193</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+      <c r="O12" s="15"/>
+      <c r="P12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1236</v>
       </c>
@@ -1569,15 +1688,26 @@
       <c r="H13" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="15"/>
-      <c r="M13" t="s">
+      <c r="I13" s="5">
+        <v>230</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5">
+        <v>1</v>
+      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1236</v>
       </c>
@@ -1602,15 +1732,26 @@
       <c r="H14" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
-      <c r="M14" t="s">
+      <c r="I14" s="5">
+        <v>228</v>
+      </c>
+      <c r="J14" s="5">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1236</v>
       </c>
@@ -1635,15 +1776,26 @@
       <c r="H15" s="8">
         <v>1</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="M15" t="s">
+      <c r="I15" s="8">
+        <v>266</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8">
+        <v>1</v>
+      </c>
+      <c r="O15" s="9"/>
+      <c r="P15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8430</v>
       </c>
@@ -1668,15 +1820,26 @@
       <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="M16" t="s">
+      <c r="I16" s="2">
+        <v>147</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>8430</v>
       </c>
@@ -1701,15 +1864,26 @@
       <c r="H17" s="5">
         <v>1</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="15"/>
-      <c r="M17" t="s">
+      <c r="I17" s="5">
+        <v>149</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1</v>
+      </c>
+      <c r="K17" s="5">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5">
+        <v>1</v>
+      </c>
+      <c r="O17" s="15"/>
+      <c r="P17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>8430</v>
       </c>
@@ -1734,15 +1908,26 @@
       <c r="H18" s="5">
         <v>1</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="15"/>
-      <c r="M18" t="s">
+      <c r="I18" s="5">
+        <v>221</v>
+      </c>
+      <c r="J18" s="5">
+        <v>1</v>
+      </c>
+      <c r="K18" s="5">
+        <v>1</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5">
+        <v>1</v>
+      </c>
+      <c r="O18" s="15"/>
+      <c r="P18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>8430</v>
       </c>
@@ -1767,15 +1952,26 @@
       <c r="H19" s="5">
         <v>1</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="15"/>
-      <c r="M19" t="s">
+      <c r="I19" s="5">
+        <v>184</v>
+      </c>
+      <c r="J19" s="5">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5">
+        <v>1</v>
+      </c>
+      <c r="O19" s="15"/>
+      <c r="P19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>8430</v>
       </c>
@@ -1800,15 +1996,26 @@
       <c r="H20" s="5">
         <v>1</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="15"/>
-      <c r="M20" t="s">
+      <c r="I20" s="5">
+        <v>155</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5">
+        <v>1</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5">
+        <v>1</v>
+      </c>
+      <c r="O20" s="15"/>
+      <c r="P20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>8430</v>
       </c>
@@ -1833,15 +2040,26 @@
       <c r="H21" s="5">
         <v>1</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="15"/>
-      <c r="M21" t="s">
+      <c r="I21" s="5">
+        <v>164</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1</v>
+      </c>
+      <c r="K21" s="5">
+        <v>1</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5">
+        <v>1</v>
+      </c>
+      <c r="O21" s="15"/>
+      <c r="P21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>8430</v>
       </c>
@@ -1866,15 +2084,26 @@
       <c r="H22" s="5">
         <v>1</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="15"/>
-      <c r="M22" t="s">
+      <c r="I22" s="5">
+        <v>200</v>
+      </c>
+      <c r="J22" s="5">
+        <v>1</v>
+      </c>
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+      <c r="O22" s="15"/>
+      <c r="P22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>8430</v>
       </c>
@@ -1896,18 +2125,27 @@
       <c r="G23" s="11">
         <v>1</v>
       </c>
-      <c r="H23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="15"/>
-      <c r="M23" t="s">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5">
+        <v>182</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5">
+        <v>1</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="15"/>
+      <c r="P23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>8430</v>
       </c>
@@ -1932,15 +2170,26 @@
       <c r="H24" s="5">
         <v>1</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="15"/>
-      <c r="M24" t="s">
+      <c r="I24" s="5">
+        <v>218</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1</v>
+      </c>
+      <c r="K24" s="5">
+        <v>1</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+      <c r="O24" s="15"/>
+      <c r="P24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>8430</v>
       </c>
@@ -1962,18 +2211,23 @@
       <c r="G25" s="11">
         <v>1</v>
       </c>
-      <c r="H25" s="5">
-        <v>1</v>
-      </c>
-      <c r="I25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5">
+        <v>212</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="15"/>
-      <c r="M25" t="s">
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5">
+        <v>1</v>
+      </c>
+      <c r="O25" s="15"/>
+      <c r="P25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>8430</v>
       </c>
@@ -1995,18 +2249,23 @@
       <c r="G26" s="11">
         <v>1</v>
       </c>
-      <c r="H26" s="5">
-        <v>1</v>
-      </c>
-      <c r="I26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5">
+        <v>226</v>
+      </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="15"/>
-      <c r="M26" t="s">
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5">
+        <v>1</v>
+      </c>
+      <c r="O26" s="15"/>
+      <c r="P26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>8430</v>
       </c>
@@ -2031,15 +2290,22 @@
       <c r="H27" s="5">
         <v>1</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="5">
+        <v>417</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="6"/>
-      <c r="M27" t="s">
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5">
+        <v>1</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>8430</v>
       </c>
@@ -2064,15 +2330,22 @@
       <c r="H28" s="5">
         <v>1</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5">
+        <v>420</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="6"/>
-      <c r="M28" t="s">
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5">
+        <v>1</v>
+      </c>
+      <c r="O28" s="6"/>
+      <c r="P28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>8430</v>
       </c>
@@ -2097,15 +2370,22 @@
       <c r="H29" s="8">
         <v>1</v>
       </c>
-      <c r="I29" s="8"/>
+      <c r="I29" s="8">
+        <v>309</v>
+      </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="9"/>
-      <c r="M29" t="s">
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8">
+        <v>1</v>
+      </c>
+      <c r="O29" s="9"/>
+      <c r="P29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>8815</v>
       </c>
@@ -2130,15 +2410,22 @@
       <c r="H30" s="2">
         <v>1</v>
       </c>
-      <c r="I30" s="2"/>
+      <c r="I30" s="2">
+        <v>213</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" t="s">
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="3"/>
+      <c r="P30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>8815</v>
       </c>
@@ -2163,15 +2450,22 @@
       <c r="H31" s="5">
         <v>1</v>
       </c>
-      <c r="I31" s="5"/>
+      <c r="I31" s="5">
+        <v>582</v>
+      </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="6"/>
-      <c r="M31" t="s">
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5">
+        <v>1</v>
+      </c>
+      <c r="O31" s="6"/>
+      <c r="P31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>8815</v>
       </c>
@@ -2196,15 +2490,22 @@
       <c r="H32" s="5">
         <v>1</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="5">
+        <v>307</v>
+      </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="6"/>
-      <c r="M32" t="s">
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5">
+        <v>1</v>
+      </c>
+      <c r="O32" s="6"/>
+      <c r="P32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>8815</v>
       </c>
@@ -2229,15 +2530,22 @@
       <c r="H33" s="5">
         <v>1</v>
       </c>
-      <c r="I33" s="5"/>
+      <c r="I33" s="5">
+        <v>326</v>
+      </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="6"/>
-      <c r="M33" t="s">
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5">
+        <v>1</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>8815</v>
       </c>
@@ -2262,15 +2570,22 @@
       <c r="H34" s="5">
         <v>1</v>
       </c>
-      <c r="I34" s="5"/>
+      <c r="I34" s="5">
+        <v>487</v>
+      </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
-      <c r="L34" s="6"/>
-      <c r="M34" t="s">
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5">
+        <v>1</v>
+      </c>
+      <c r="O34" s="6"/>
+      <c r="P34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>8815</v>
       </c>
@@ -2292,18 +2607,23 @@
       <c r="G35" s="5">
         <v>1</v>
       </c>
-      <c r="H35" s="5">
-        <v>1</v>
-      </c>
-      <c r="I35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5">
+        <v>334</v>
+      </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
-      <c r="L35" s="6"/>
-      <c r="M35" t="s">
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5">
+        <v>1</v>
+      </c>
+      <c r="O35" s="6"/>
+      <c r="P35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>8815</v>
       </c>
@@ -2328,15 +2648,22 @@
       <c r="H36" s="5">
         <v>1</v>
       </c>
-      <c r="I36" s="5"/>
+      <c r="I36" s="5">
+        <v>280</v>
+      </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
-      <c r="L36" s="6"/>
-      <c r="M36" t="s">
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5">
+        <v>1</v>
+      </c>
+      <c r="O36" s="6"/>
+      <c r="P36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>8815</v>
       </c>
@@ -2361,15 +2688,22 @@
       <c r="H37" s="5">
         <v>1</v>
       </c>
-      <c r="I37" s="5"/>
+      <c r="I37" s="5">
+        <v>304</v>
+      </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
-      <c r="L37" s="6"/>
-      <c r="M37" t="s">
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5">
+        <v>1</v>
+      </c>
+      <c r="O37" s="6"/>
+      <c r="P37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>8815</v>
       </c>
@@ -2394,15 +2728,22 @@
       <c r="H38" s="5">
         <v>1</v>
       </c>
-      <c r="I38" s="5"/>
+      <c r="I38" s="5">
+        <v>286</v>
+      </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="6"/>
-      <c r="M38" t="s">
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5">
+        <v>1</v>
+      </c>
+      <c r="O38" s="6"/>
+      <c r="P38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>8815</v>
       </c>
@@ -2427,15 +2768,22 @@
       <c r="H39" s="5">
         <v>1</v>
       </c>
-      <c r="I39" s="5"/>
+      <c r="I39" s="5">
+        <v>321</v>
+      </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="6"/>
-      <c r="M39" t="s">
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5">
+        <v>1</v>
+      </c>
+      <c r="O39" s="6"/>
+      <c r="P39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>8815</v>
       </c>
@@ -2457,18 +2805,23 @@
       <c r="G40" s="5">
         <v>1</v>
       </c>
-      <c r="H40" s="5">
-        <v>1</v>
-      </c>
-      <c r="I40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5">
+        <v>128</v>
+      </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="6"/>
-      <c r="M40" t="s">
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5">
+        <v>1</v>
+      </c>
+      <c r="O40" s="6"/>
+      <c r="P40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>8815</v>
       </c>
@@ -2493,15 +2846,22 @@
       <c r="H41" s="5">
         <v>1</v>
       </c>
-      <c r="I41" s="5"/>
+      <c r="I41" s="5">
+        <v>349</v>
+      </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="6"/>
-      <c r="M41" t="s">
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5">
+        <v>1</v>
+      </c>
+      <c r="O41" s="6"/>
+      <c r="P41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>8815</v>
       </c>
@@ -2529,12 +2889,15 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="6"/>
-      <c r="M42" t="s">
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="6"/>
+      <c r="P42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
         <v>8815</v>
       </c>
@@ -2562,12 +2925,15 @@
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
-      <c r="L43" s="9"/>
-      <c r="M43" t="s">
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="9"/>
+      <c r="P43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>8803</v>
       </c>
@@ -2595,12 +2961,15 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="3"/>
-      <c r="M44" t="s">
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="3"/>
+      <c r="P44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>8803</v>
       </c>
@@ -2628,12 +2997,15 @@
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
-      <c r="L45" s="6"/>
-      <c r="M45" t="s">
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="6"/>
+      <c r="P45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>8803</v>
       </c>
@@ -2661,12 +3033,15 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
-      <c r="L46" s="6"/>
-      <c r="M46" t="s">
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="6"/>
+      <c r="P46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>8803</v>
       </c>
@@ -2694,12 +3069,15 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
-      <c r="L47" s="6"/>
-      <c r="M47" t="s">
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="6"/>
+      <c r="P47" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>8803</v>
       </c>
@@ -2727,12 +3105,15 @@
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
-      <c r="L48" s="6"/>
-      <c r="M48" t="s">
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="6"/>
+      <c r="P48" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>8803</v>
       </c>
@@ -2760,12 +3141,15 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
-      <c r="L49" s="6"/>
-      <c r="M49" t="s">
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="6"/>
+      <c r="P49" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>8803</v>
       </c>
@@ -2787,18 +3171,19 @@
       <c r="G50" s="5">
         <v>1</v>
       </c>
-      <c r="H50" s="5">
-        <v>1</v>
-      </c>
+      <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="6"/>
-      <c r="M50" t="s">
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="6"/>
+      <c r="P50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>8803</v>
       </c>
@@ -2826,12 +3211,15 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="6"/>
-      <c r="M51" t="s">
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="6"/>
+      <c r="P51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>8803</v>
       </c>
@@ -2859,12 +3247,15 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="6"/>
-      <c r="M52" t="s">
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="6"/>
+      <c r="P52" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>8803</v>
       </c>
@@ -2892,12 +3283,15 @@
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
-      <c r="L53" s="6"/>
-      <c r="M53" t="s">
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="6"/>
+      <c r="P53" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>8803</v>
       </c>
@@ -2925,12 +3319,15 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
-      <c r="L54" s="6"/>
-      <c r="M54" t="s">
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="6"/>
+      <c r="P54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>8803</v>
       </c>
@@ -2958,12 +3355,15 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
-      <c r="L55" s="6"/>
-      <c r="M55" t="s">
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="6"/>
+      <c r="P55" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>8803</v>
       </c>
@@ -2991,12 +3391,15 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
-      <c r="L56" s="6"/>
-      <c r="M56" t="s">
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="6"/>
+      <c r="P56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>8803</v>
       </c>
@@ -3024,12 +3427,15 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
-      <c r="L57" s="6"/>
-      <c r="M57" t="s">
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="6"/>
+      <c r="P57" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
         <v>8803</v>
       </c>
@@ -3057,12 +3463,15 @@
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
-      <c r="L58" s="9"/>
-      <c r="M58" t="s">
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="9"/>
+      <c r="P58" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>1208</v>
       </c>
@@ -3090,12 +3499,15 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
-      <c r="L59" s="3"/>
-      <c r="M59" t="s">
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="3"/>
+      <c r="P59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>1208</v>
       </c>
@@ -3123,12 +3535,15 @@
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
-      <c r="L60" s="6"/>
-      <c r="M60" t="s">
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="6"/>
+      <c r="P60" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>1208</v>
       </c>
@@ -3156,12 +3571,15 @@
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
-      <c r="L61" s="6"/>
-      <c r="M61" t="s">
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="6"/>
+      <c r="P61" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>1208</v>
       </c>
@@ -3189,12 +3607,15 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
-      <c r="L62" s="6"/>
-      <c r="M62" t="s">
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="6"/>
+      <c r="P62" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>1208</v>
       </c>
@@ -3222,12 +3643,15 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
-      <c r="L63" s="6"/>
-      <c r="M63" t="s">
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="6"/>
+      <c r="P63" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>1208</v>
       </c>
@@ -3255,12 +3679,15 @@
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
-      <c r="L64" s="6"/>
-      <c r="M64" t="s">
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="6"/>
+      <c r="P64" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>1208</v>
       </c>
@@ -3288,12 +3715,15 @@
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
-      <c r="L65" s="6"/>
-      <c r="M65" t="s">
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="6"/>
+      <c r="P65" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>1208</v>
       </c>
@@ -3321,12 +3751,15 @@
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
-      <c r="L66" s="6"/>
-      <c r="M66" t="s">
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="6"/>
+      <c r="P66" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>1208</v>
       </c>
@@ -3354,12 +3787,15 @@
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
-      <c r="L67" s="6"/>
-      <c r="M67" t="s">
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="6"/>
+      <c r="P67" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>1208</v>
       </c>
@@ -3387,12 +3823,15 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
-      <c r="L68" s="6"/>
-      <c r="M68" t="s">
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="6"/>
+      <c r="P68" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>1208</v>
       </c>
@@ -3420,12 +3859,15 @@
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
-      <c r="L69" s="6"/>
-      <c r="M69" t="s">
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="6"/>
+      <c r="P69" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>1208</v>
       </c>
@@ -3447,18 +3889,19 @@
       <c r="G70" s="5">
         <v>1</v>
       </c>
-      <c r="H70" s="5">
-        <v>1</v>
-      </c>
+      <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
-      <c r="L70" s="6"/>
-      <c r="M70" t="s">
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="6"/>
+      <c r="P70" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>1208</v>
       </c>
@@ -3486,12 +3929,15 @@
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
-      <c r="L71" s="6"/>
-      <c r="M71" t="s">
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="6"/>
+      <c r="P71" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
         <v>1208</v>
       </c>
@@ -3519,12 +3965,15 @@
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
-      <c r="L72" s="9"/>
-      <c r="M72" t="s">
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="9"/>
+      <c r="P72" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>1793</v>
       </c>
@@ -3552,12 +4001,15 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
-      <c r="L73" s="3"/>
-      <c r="M73" t="s">
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="3"/>
+      <c r="P73" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>1793</v>
       </c>
@@ -3585,12 +4037,15 @@
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
-      <c r="L74" s="6"/>
-      <c r="M74" t="s">
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="6"/>
+      <c r="P74" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>1793</v>
       </c>
@@ -3618,12 +4073,15 @@
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
-      <c r="L75" s="6"/>
-      <c r="M75" t="s">
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="6"/>
+      <c r="P75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>1793</v>
       </c>
@@ -3651,12 +4109,15 @@
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
-      <c r="L76" s="6"/>
-      <c r="M76" t="s">
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="6"/>
+      <c r="P76" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>1793</v>
       </c>
@@ -3684,12 +4145,15 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
-      <c r="L77" s="6"/>
-      <c r="M77" t="s">
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="6"/>
+      <c r="P77" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>1793</v>
       </c>
@@ -3717,12 +4181,15 @@
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
-      <c r="L78" s="6"/>
-      <c r="M78" t="s">
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="6"/>
+      <c r="P78" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>1793</v>
       </c>
@@ -3750,12 +4217,15 @@
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
-      <c r="L79" s="6"/>
-      <c r="M79" t="s">
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="6"/>
+      <c r="P79" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>1793</v>
       </c>
@@ -3783,12 +4253,15 @@
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
-      <c r="L80" s="6"/>
-      <c r="M80" t="s">
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="6"/>
+      <c r="P80" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
         <v>1793</v>
       </c>
@@ -3816,12 +4289,15 @@
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
-      <c r="L81" s="6"/>
-      <c r="M81" t="s">
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5"/>
+      <c r="O81" s="6"/>
+      <c r="P81" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>1793</v>
       </c>
@@ -3849,12 +4325,15 @@
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
-      <c r="L82" s="6"/>
-      <c r="M82" t="s">
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5"/>
+      <c r="O82" s="6"/>
+      <c r="P82" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
         <v>1793</v>
       </c>
@@ -3882,12 +4361,15 @@
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
-      <c r="L83" s="6"/>
-      <c r="M83" t="s">
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="6"/>
+      <c r="P83" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>1793</v>
       </c>
@@ -3915,12 +4397,15 @@
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
-      <c r="L84" s="6"/>
-      <c r="M84" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="6"/>
+      <c r="P84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
         <v>1793</v>
       </c>
@@ -3948,12 +4433,15 @@
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
-      <c r="L85" s="6"/>
-      <c r="M85" t="s">
+      <c r="L85" s="5"/>
+      <c r="M85" s="5"/>
+      <c r="N85" s="5"/>
+      <c r="O85" s="6"/>
+      <c r="P85" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
         <v>1793</v>
       </c>
@@ -3981,8 +4469,11 @@
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
       <c r="K86" s="8"/>
-      <c r="L86" s="9"/>
-      <c r="M86" t="s">
+      <c r="L86" s="8"/>
+      <c r="M86" s="8"/>
+      <c r="N86" s="8"/>
+      <c r="O86" s="9"/>
+      <c r="P86" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated spredsheet with marked_red sessions
</commit_message>
<xml_diff>
--- a/new_data/pathways.xlsx
+++ b/new_data/pathways.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="40">
   <si>
     <t>mouse</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>hs_t</t>
+  </si>
+  <si>
+    <t>PV</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B54" workbookViewId="0">
+      <selection activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,9 +1130,10 @@
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1178,8 +1182,11 @@
       <c r="P1" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1236</v>
       </c>
@@ -1213,7 +1220,9 @@
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2">
         <v>1</v>
@@ -1222,8 +1231,11 @@
       <c r="P2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1236</v>
       </c>
@@ -1266,8 +1278,11 @@
       <c r="P3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1236</v>
       </c>
@@ -1310,8 +1325,11 @@
       <c r="P4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1236</v>
       </c>
@@ -1354,8 +1372,11 @@
       <c r="P5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1236</v>
       </c>
@@ -1398,8 +1419,11 @@
       <c r="P6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1236</v>
       </c>
@@ -1442,8 +1466,11 @@
       <c r="P7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1236</v>
       </c>
@@ -1486,8 +1513,11 @@
       <c r="P8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1236</v>
       </c>
@@ -1530,8 +1560,11 @@
       <c r="P9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1236</v>
       </c>
@@ -1574,8 +1607,11 @@
       <c r="P10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1236</v>
       </c>
@@ -1618,8 +1654,11 @@
       <c r="P11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1236</v>
       </c>
@@ -1662,8 +1701,11 @@
       <c r="P12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1236</v>
       </c>
@@ -1706,8 +1748,11 @@
       <c r="P13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1236</v>
       </c>
@@ -1750,8 +1795,11 @@
       <c r="P14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1236</v>
       </c>
@@ -1794,8 +1842,11 @@
       <c r="P15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8430</v>
       </c>
@@ -1838,8 +1889,11 @@
       <c r="P16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>8430</v>
       </c>
@@ -1882,8 +1936,11 @@
       <c r="P17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>8430</v>
       </c>
@@ -1926,8 +1983,11 @@
       <c r="P18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>8430</v>
       </c>
@@ -1970,8 +2030,11 @@
       <c r="P19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>8430</v>
       </c>
@@ -2014,8 +2077,11 @@
       <c r="P20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>8430</v>
       </c>
@@ -2058,8 +2124,11 @@
       <c r="P21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>8430</v>
       </c>
@@ -2102,8 +2171,11 @@
       <c r="P22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>8430</v>
       </c>
@@ -2144,8 +2216,11 @@
       <c r="P23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>8430</v>
       </c>
@@ -2188,8 +2263,11 @@
       <c r="P24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>8430</v>
       </c>
@@ -2215,8 +2293,12 @@
       <c r="I25" s="5">
         <v>212</v>
       </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="J25" s="5">
+        <v>1</v>
+      </c>
+      <c r="K25" s="5">
+        <v>1</v>
+      </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5">
@@ -2226,8 +2308,11 @@
       <c r="P25" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>8430</v>
       </c>
@@ -2253,8 +2338,12 @@
       <c r="I26" s="5">
         <v>226</v>
       </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="J26" s="5">
+        <v>1</v>
+      </c>
+      <c r="K26" s="5">
+        <v>1</v>
+      </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5">
@@ -2264,8 +2353,11 @@
       <c r="P26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>8430</v>
       </c>
@@ -2293,8 +2385,12 @@
       <c r="I27" s="5">
         <v>417</v>
       </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="J27" s="5">
+        <v>1</v>
+      </c>
+      <c r="K27" s="5">
+        <v>1</v>
+      </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5">
@@ -2304,8 +2400,11 @@
       <c r="P27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>8430</v>
       </c>
@@ -2333,8 +2432,12 @@
       <c r="I28" s="5">
         <v>420</v>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
+      <c r="K28" s="5">
+        <v>1</v>
+      </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5">
@@ -2344,8 +2447,11 @@
       <c r="P28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>8430</v>
       </c>
@@ -2373,8 +2479,12 @@
       <c r="I29" s="8">
         <v>309</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="J29" s="8">
+        <v>1</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1</v>
+      </c>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8">
@@ -2384,8 +2494,11 @@
       <c r="P29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>8815</v>
       </c>
@@ -2413,8 +2526,12 @@
       <c r="I30" s="2">
         <v>213</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2">
@@ -2424,8 +2541,11 @@
       <c r="P30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>8815</v>
       </c>
@@ -2453,8 +2573,12 @@
       <c r="I31" s="5">
         <v>582</v>
       </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5">
+        <v>1</v>
+      </c>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5">
@@ -2464,8 +2588,11 @@
       <c r="P31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>8815</v>
       </c>
@@ -2493,8 +2620,12 @@
       <c r="I32" s="5">
         <v>307</v>
       </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
+      <c r="J32" s="5">
+        <v>1</v>
+      </c>
+      <c r="K32" s="5">
+        <v>1</v>
+      </c>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
       <c r="N32" s="5">
@@ -2504,8 +2635,11 @@
       <c r="P32" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>8815</v>
       </c>
@@ -2533,8 +2667,12 @@
       <c r="I33" s="5">
         <v>326</v>
       </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
+      <c r="J33" s="5">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5">
+        <v>1</v>
+      </c>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5">
@@ -2544,8 +2682,11 @@
       <c r="P33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>8815</v>
       </c>
@@ -2573,8 +2714,12 @@
       <c r="I34" s="5">
         <v>487</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="J34" s="5">
+        <v>1</v>
+      </c>
+      <c r="K34" s="5">
+        <v>1</v>
+      </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
       <c r="N34" s="5">
@@ -2584,8 +2729,11 @@
       <c r="P34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>8815</v>
       </c>
@@ -2611,8 +2759,12 @@
       <c r="I35" s="5">
         <v>334</v>
       </c>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+      <c r="J35" s="5">
+        <v>1</v>
+      </c>
+      <c r="K35" s="5">
+        <v>1</v>
+      </c>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5">
@@ -2622,8 +2774,11 @@
       <c r="P35" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>8815</v>
       </c>
@@ -2651,8 +2806,12 @@
       <c r="I36" s="5">
         <v>280</v>
       </c>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+      <c r="J36" s="5">
+        <v>1</v>
+      </c>
+      <c r="K36" s="5">
+        <v>1</v>
+      </c>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5">
@@ -2662,8 +2821,11 @@
       <c r="P36" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>8815</v>
       </c>
@@ -2691,8 +2853,12 @@
       <c r="I37" s="5">
         <v>304</v>
       </c>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
+      <c r="J37" s="5">
+        <v>1</v>
+      </c>
+      <c r="K37" s="5">
+        <v>1</v>
+      </c>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
       <c r="N37" s="5">
@@ -2702,8 +2868,11 @@
       <c r="P37" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>8815</v>
       </c>
@@ -2731,8 +2900,12 @@
       <c r="I38" s="5">
         <v>286</v>
       </c>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
+      <c r="J38" s="5">
+        <v>1</v>
+      </c>
+      <c r="K38" s="5">
+        <v>1</v>
+      </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="5">
@@ -2742,8 +2915,11 @@
       <c r="P38" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>8815</v>
       </c>
@@ -2771,8 +2947,12 @@
       <c r="I39" s="5">
         <v>321</v>
       </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
+      <c r="J39" s="5">
+        <v>1</v>
+      </c>
+      <c r="K39" s="5">
+        <v>1</v>
+      </c>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5">
@@ -2782,8 +2962,11 @@
       <c r="P39" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>8815</v>
       </c>
@@ -2809,8 +2992,12 @@
       <c r="I40" s="5">
         <v>128</v>
       </c>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
+      <c r="J40" s="5">
+        <v>1</v>
+      </c>
+      <c r="K40" s="5">
+        <v>1</v>
+      </c>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5">
@@ -2820,8 +3007,11 @@
       <c r="P40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>8815</v>
       </c>
@@ -2849,8 +3039,12 @@
       <c r="I41" s="5">
         <v>349</v>
       </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
+      <c r="J41" s="5">
+        <v>1</v>
+      </c>
+      <c r="K41" s="5">
+        <v>1</v>
+      </c>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
       <c r="N41" s="5">
@@ -2860,8 +3054,11 @@
       <c r="P41" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>8815</v>
       </c>
@@ -2887,8 +3084,12 @@
         <v>1</v>
       </c>
       <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+      <c r="J42" s="5">
+        <v>1</v>
+      </c>
+      <c r="K42" s="5">
+        <v>1</v>
+      </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
@@ -2896,8 +3097,11 @@
       <c r="P42" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
         <v>8815</v>
       </c>
@@ -2923,8 +3127,12 @@
         <v>1</v>
       </c>
       <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
+      <c r="J43" s="8">
+        <v>1</v>
+      </c>
+      <c r="K43" s="8">
+        <v>1</v>
+      </c>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
@@ -2932,8 +3140,11 @@
       <c r="P43" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>8803</v>
       </c>
@@ -2959,8 +3170,12 @@
         <v>1</v>
       </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+      <c r="J44" s="2">
+        <v>1</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1</v>
+      </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -2968,8 +3183,11 @@
       <c r="P44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>8803</v>
       </c>
@@ -2995,8 +3213,12 @@
         <v>1</v>
       </c>
       <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
+      <c r="J45" s="5">
+        <v>1</v>
+      </c>
+      <c r="K45" s="5">
+        <v>1</v>
+      </c>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3004,8 +3226,11 @@
       <c r="P45" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>8803</v>
       </c>
@@ -3031,8 +3256,12 @@
         <v>1</v>
       </c>
       <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
+      <c r="J46" s="5">
+        <v>1</v>
+      </c>
+      <c r="K46" s="5">
+        <v>1</v>
+      </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3040,8 +3269,11 @@
       <c r="P46" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>8803</v>
       </c>
@@ -3067,8 +3299,12 @@
         <v>1</v>
       </c>
       <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
+      <c r="J47" s="5">
+        <v>1</v>
+      </c>
+      <c r="K47" s="5">
+        <v>1</v>
+      </c>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
@@ -3076,8 +3312,11 @@
       <c r="P47" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>8803</v>
       </c>
@@ -3103,8 +3342,12 @@
         <v>1</v>
       </c>
       <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
+      <c r="J48" s="5">
+        <v>1</v>
+      </c>
+      <c r="K48" s="5">
+        <v>1</v>
+      </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
@@ -3112,8 +3355,11 @@
       <c r="P48" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>8803</v>
       </c>
@@ -3139,8 +3385,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
+      <c r="J49" s="5">
+        <v>1</v>
+      </c>
+      <c r="K49" s="5">
+        <v>1</v>
+      </c>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
@@ -3148,8 +3398,11 @@
       <c r="P49" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>8803</v>
       </c>
@@ -3173,8 +3426,12 @@
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
+      <c r="J50" s="5">
+        <v>1</v>
+      </c>
+      <c r="K50" s="5">
+        <v>1</v>
+      </c>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
@@ -3182,8 +3439,11 @@
       <c r="P50" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>8803</v>
       </c>
@@ -3209,8 +3469,12 @@
         <v>1</v>
       </c>
       <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
+      <c r="J51" s="5">
+        <v>1</v>
+      </c>
+      <c r="K51" s="5">
+        <v>1</v>
+      </c>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
@@ -3218,8 +3482,11 @@
       <c r="P51" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>8803</v>
       </c>
@@ -3245,8 +3512,12 @@
         <v>1</v>
       </c>
       <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
+      <c r="J52" s="5">
+        <v>1</v>
+      </c>
+      <c r="K52" s="5">
+        <v>1</v>
+      </c>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
@@ -3254,8 +3525,11 @@
       <c r="P52" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>8803</v>
       </c>
@@ -3281,8 +3555,12 @@
         <v>1</v>
       </c>
       <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
+      <c r="J53" s="5">
+        <v>1</v>
+      </c>
+      <c r="K53" s="5">
+        <v>1</v>
+      </c>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
@@ -3290,8 +3568,11 @@
       <c r="P53" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>8803</v>
       </c>
@@ -3317,8 +3598,12 @@
         <v>1</v>
       </c>
       <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
+      <c r="J54" s="5">
+        <v>1</v>
+      </c>
+      <c r="K54" s="5">
+        <v>1</v>
+      </c>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
@@ -3326,8 +3611,11 @@
       <c r="P54" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>8803</v>
       </c>
@@ -3353,8 +3641,12 @@
         <v>1</v>
       </c>
       <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
+      <c r="J55" s="5">
+        <v>1</v>
+      </c>
+      <c r="K55" s="5">
+        <v>1</v>
+      </c>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
@@ -3362,8 +3654,11 @@
       <c r="P55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>8803</v>
       </c>
@@ -3389,8 +3684,12 @@
         <v>1</v>
       </c>
       <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
+      <c r="J56" s="5">
+        <v>1</v>
+      </c>
+      <c r="K56" s="5">
+        <v>1</v>
+      </c>
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
@@ -3398,8 +3697,11 @@
       <c r="P56" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>8803</v>
       </c>
@@ -3425,8 +3727,12 @@
         <v>1</v>
       </c>
       <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
+      <c r="J57" s="5">
+        <v>1</v>
+      </c>
+      <c r="K57" s="5">
+        <v>1</v>
+      </c>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
@@ -3434,8 +3740,11 @@
       <c r="P57" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
         <v>8803</v>
       </c>
@@ -3461,8 +3770,12 @@
         <v>1</v>
       </c>
       <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
+      <c r="J58" s="8">
+        <v>1</v>
+      </c>
+      <c r="K58" s="8">
+        <v>1</v>
+      </c>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
@@ -3470,8 +3783,11 @@
       <c r="P58" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>1208</v>
       </c>
@@ -3497,8 +3813,12 @@
         <v>1</v>
       </c>
       <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+      <c r="J59" s="2">
+        <v>1</v>
+      </c>
+      <c r="K59" s="2">
+        <v>1</v>
+      </c>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3506,8 +3826,11 @@
       <c r="P59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>1208</v>
       </c>
@@ -3533,8 +3856,12 @@
         <v>1</v>
       </c>
       <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
+      <c r="J60" s="5">
+        <v>1</v>
+      </c>
+      <c r="K60" s="5">
+        <v>1</v>
+      </c>
       <c r="L60" s="5"/>
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
@@ -3542,8 +3869,11 @@
       <c r="P60" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>1208</v>
       </c>
@@ -3569,8 +3899,12 @@
         <v>1</v>
       </c>
       <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
+      <c r="J61" s="5">
+        <v>1</v>
+      </c>
+      <c r="K61" s="5">
+        <v>1</v>
+      </c>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
       <c r="N61" s="5"/>
@@ -3578,8 +3912,11 @@
       <c r="P61" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>1208</v>
       </c>
@@ -3605,8 +3942,12 @@
         <v>1</v>
       </c>
       <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
+      <c r="J62" s="5">
+        <v>1</v>
+      </c>
+      <c r="K62" s="5">
+        <v>1</v>
+      </c>
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
@@ -3614,8 +3955,11 @@
       <c r="P62" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>1208</v>
       </c>
@@ -3641,8 +3985,12 @@
         <v>1</v>
       </c>
       <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
+      <c r="J63" s="5">
+        <v>1</v>
+      </c>
+      <c r="K63" s="5">
+        <v>1</v>
+      </c>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
@@ -3650,8 +3998,11 @@
       <c r="P63" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>1208</v>
       </c>
@@ -3677,8 +4028,12 @@
         <v>1</v>
       </c>
       <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
+      <c r="J64" s="5">
+        <v>1</v>
+      </c>
+      <c r="K64" s="5">
+        <v>1</v>
+      </c>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -3686,8 +4041,11 @@
       <c r="P64" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>1208</v>
       </c>
@@ -3713,8 +4071,12 @@
         <v>1</v>
       </c>
       <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
+      <c r="J65" s="5">
+        <v>1</v>
+      </c>
+      <c r="K65" s="5">
+        <v>1</v>
+      </c>
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
@@ -3722,8 +4084,11 @@
       <c r="P65" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>1208</v>
       </c>
@@ -3749,8 +4114,12 @@
         <v>1</v>
       </c>
       <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
+      <c r="J66" s="5">
+        <v>1</v>
+      </c>
+      <c r="K66" s="5">
+        <v>1</v>
+      </c>
       <c r="L66" s="5"/>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
@@ -3758,8 +4127,11 @@
       <c r="P66" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>1208</v>
       </c>
@@ -3785,8 +4157,12 @@
         <v>1</v>
       </c>
       <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
+      <c r="J67" s="5">
+        <v>1</v>
+      </c>
+      <c r="K67" s="5">
+        <v>1</v>
+      </c>
       <c r="L67" s="5"/>
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
@@ -3794,8 +4170,11 @@
       <c r="P67" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>1208</v>
       </c>
@@ -3821,8 +4200,12 @@
         <v>1</v>
       </c>
       <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
+      <c r="J68" s="5">
+        <v>1</v>
+      </c>
+      <c r="K68" s="5">
+        <v>1</v>
+      </c>
       <c r="L68" s="5"/>
       <c r="M68" s="5"/>
       <c r="N68" s="5"/>
@@ -3830,8 +4213,11 @@
       <c r="P68" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>1208</v>
       </c>
@@ -3857,8 +4243,12 @@
         <v>1</v>
       </c>
       <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
+      <c r="J69" s="5">
+        <v>1</v>
+      </c>
+      <c r="K69" s="5">
+        <v>1</v>
+      </c>
       <c r="L69" s="5"/>
       <c r="M69" s="5"/>
       <c r="N69" s="5"/>
@@ -3866,8 +4256,11 @@
       <c r="P69" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>1208</v>
       </c>
@@ -3891,8 +4284,12 @@
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
+      <c r="J70" s="5">
+        <v>1</v>
+      </c>
+      <c r="K70" s="5">
+        <v>1</v>
+      </c>
       <c r="L70" s="5"/>
       <c r="M70" s="5"/>
       <c r="N70" s="5"/>
@@ -3900,8 +4297,11 @@
       <c r="P70" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>1208</v>
       </c>
@@ -3927,8 +4327,12 @@
         <v>1</v>
       </c>
       <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
+      <c r="J71" s="5">
+        <v>1</v>
+      </c>
+      <c r="K71" s="5">
+        <v>1</v>
+      </c>
       <c r="L71" s="5"/>
       <c r="M71" s="5"/>
       <c r="N71" s="5"/>
@@ -3936,8 +4340,11 @@
       <c r="P71" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
         <v>1208</v>
       </c>
@@ -3963,8 +4370,12 @@
         <v>1</v>
       </c>
       <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
+      <c r="J72" s="8">
+        <v>1</v>
+      </c>
+      <c r="K72" s="8">
+        <v>1</v>
+      </c>
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
       <c r="N72" s="8"/>
@@ -3972,8 +4383,11 @@
       <c r="P72" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>1793</v>
       </c>
@@ -3999,8 +4413,12 @@
         <v>1</v>
       </c>
       <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
+      <c r="J73" s="2">
+        <v>1</v>
+      </c>
+      <c r="K73" s="2">
+        <v>1</v>
+      </c>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4008,8 +4426,11 @@
       <c r="P73" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>1793</v>
       </c>
@@ -4044,8 +4465,11 @@
       <c r="P74" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>1793</v>
       </c>
@@ -4080,8 +4504,11 @@
       <c r="P75" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>1793</v>
       </c>
@@ -4116,8 +4543,11 @@
       <c r="P76" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>1793</v>
       </c>
@@ -4152,8 +4582,11 @@
       <c r="P77" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>1793</v>
       </c>
@@ -4188,8 +4621,11 @@
       <c r="P78" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>1793</v>
       </c>
@@ -4224,8 +4660,11 @@
       <c r="P79" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>1793</v>
       </c>
@@ -4260,8 +4699,11 @@
       <c r="P80" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
         <v>1793</v>
       </c>
@@ -4296,8 +4738,11 @@
       <c r="P81" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>1793</v>
       </c>
@@ -4332,8 +4777,11 @@
       <c r="P82" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
         <v>1793</v>
       </c>
@@ -4368,8 +4816,11 @@
       <c r="P83" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>1793</v>
       </c>
@@ -4404,8 +4855,11 @@
       <c r="P84" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
         <v>1793</v>
       </c>
@@ -4440,8 +4894,11 @@
       <c r="P85" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
         <v>1793</v>
       </c>
@@ -4476,6 +4933,9 @@
       <c r="P86" t="s">
         <v>24</v>
       </c>
+      <c r="Q86">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>